<commit_message>
LOD final working version
Full working LOD version for vol_name, vol_uuid,svm_name,type,state,IOPS,SnapMirror,CIFS/NFS,Quota/Qtree
</commit_message>
<xml_diff>
--- a/VolumeDetails.xlsx
+++ b/VolumeDetails.xlsx
@@ -10,6 +10,7 @@
     <sheet name="VolDetails" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="NFS Connected Clients" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Qtree and Quota" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="CIFS Connected Clients" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -554,28 +555,28 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>402</v>
+        <v>454</v>
       </c>
       <c r="H2" t="n">
         <v>20</v>
       </c>
       <c r="I2" t="n">
-        <v>2951</v>
+        <v>12030</v>
       </c>
       <c r="J2" t="n">
-        <v>3373</v>
+        <v>12504</v>
       </c>
       <c r="K2" t="n">
-        <v>6929920</v>
+        <v>6993408</v>
       </c>
       <c r="L2" t="n">
         <v>86016</v>
       </c>
       <c r="M2" t="n">
-        <v>25324</v>
+        <v>98904</v>
       </c>
       <c r="N2" t="n">
-        <v>7041260</v>
+        <v>7178328</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -625,28 +626,28 @@
         </is>
       </c>
       <c r="G3" t="n">
-        <v>86</v>
+        <v>138</v>
       </c>
       <c r="H3" t="n">
         <v>38</v>
       </c>
       <c r="I3" t="n">
-        <v>2952</v>
+        <v>12031</v>
       </c>
       <c r="J3" t="n">
-        <v>3076</v>
+        <v>12207</v>
       </c>
       <c r="K3" t="n">
-        <v>2055680</v>
+        <v>2119168</v>
       </c>
       <c r="L3" t="n">
         <v>4034560</v>
       </c>
       <c r="M3" t="n">
-        <v>25336</v>
+        <v>98916</v>
       </c>
       <c r="N3" t="n">
-        <v>6115576</v>
+        <v>6252644</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -696,28 +697,28 @@
         </is>
       </c>
       <c r="G4" t="n">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="H4" t="n">
         <v>19</v>
       </c>
       <c r="I4" t="n">
-        <v>2950</v>
+        <v>12029</v>
       </c>
       <c r="J4" t="n">
-        <v>3043</v>
+        <v>12174</v>
       </c>
       <c r="K4" t="n">
-        <v>1359360</v>
+        <v>1422848</v>
       </c>
       <c r="L4" t="n">
         <v>77824</v>
       </c>
       <c r="M4" t="n">
-        <v>25288</v>
+        <v>98868</v>
       </c>
       <c r="N4" t="n">
-        <v>1462472</v>
+        <v>1599540</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -943,6 +944,77 @@
         </is>
       </c>
       <c r="Q7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NetApp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1ac33897-7117-11ec-939b-005056b0f708</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>svm1_cluster2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>online</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>rw</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>/NetApp</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="Q8" t="inlineStr">
         <is>
           <t>NA</t>
         </is>
@@ -959,7 +1031,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1046,6 +1118,18 @@
         </is>
       </c>
       <c r="B7" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NetApp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>[]</t>
         </is>
@@ -1062,7 +1146,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1090,7 +1174,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> id 0 with no Qtree/Quota</t>
+          <t xml:space="preserve"> id 0 with no Qtree/Quota, Qtree proj1 with Quota of 12.0 GB, Qtree proj2,proj3 with No Quota</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1222,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> id 0 with no Qtree/Quota</t>
+          <t xml:space="preserve"> id 0 with no Qtree/Quota, Qtree proj1 with No Quota, Qtree proj2,proj3 with No Quota</t>
         </is>
       </c>
     </row>
@@ -1151,6 +1235,199 @@
       <c r="B7" t="inlineStr">
         <is>
           <t xml:space="preserve"> id 0 with no Qtree/Quota</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NetApp</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> id 0 with no Qtree/Quota, Qtree Ntap1 with No Quota, Qtree Ntap2 with No Quota, Qtree Ntap3 with No Quota</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Volume name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>No. of CIFS Shares</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CIFS Shares List</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ACL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>sql1_db1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sql1_log</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sql1_system_db</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>svm1_cluster1_root</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sql1_db1_dest</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sql1_log_dest</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NetApp</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>['ntap1', 'ntap2', 'ntap3']</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>['CIFS Share ntap1 has Permission to Everyone with full_control access', 'CIFS Share ntap2 has Permission to Everyone with full_control access', 'CIFS Share ntap3 has Permission to Everyone with full_control access']</t>
         </is>
       </c>
     </row>

</xml_diff>